<commit_message>
commit update code vss
</commit_message>
<xml_diff>
--- a/addons/custom/purchase_request/static/src/xlsx/template_pr.xlsx
+++ b/addons/custom/purchase_request/static/src/xlsx/template_pr.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECT\erp_forlife\custom_addons\purchase_request\static\src\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\odoo1_6\erp_forlife\custom_addons\purchase_request\static\src\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C670069D-6CF4-4AD1-8CBA-64A74CBB6664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31050" yWindow="4395" windowWidth="22425" windowHeight="11280"/>
+    <workbookView xWindow="32025" yWindow="1200" windowWidth="25545" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Yêu cầu mua hàng" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -24,54 +25,78 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>Department</t>
-  </si>
-  <si>
-    <t>Request date</t>
-  </si>
-  <si>
-    <t>Expected Arrival</t>
-  </si>
-  <si>
-    <t>Order Lines/Product</t>
-  </si>
-  <si>
-    <t>Order Lines/Asset description</t>
-  </si>
-  <si>
-    <t>Order Lines/Quantity Purchase</t>
-  </si>
-  <si>
-    <t>Order Lines/Exchange Quantity</t>
-  </si>
-  <si>
-    <t>Order Lines/UOM Purchase</t>
-  </si>
-  <si>
-    <t>Order Lines/Production Order Code</t>
-  </si>
-  <si>
-    <t>Order Lines/Request date</t>
-  </si>
-  <si>
-    <t>Order Lines/Quantity Order</t>
-  </si>
-  <si>
-    <t>User request</t>
-  </si>
-  <si>
-    <t>Order Lines/Type</t>
-  </si>
-  <si>
-    <t>Order Lines/Vendor</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+  <si>
+    <t>Người yêu cầu</t>
+  </si>
+  <si>
+    <t>Phòng/ban</t>
+  </si>
+  <si>
+    <t>Mã vụ việc</t>
+  </si>
+  <si>
+    <t>Lệnh sản xuất</t>
+  </si>
+  <si>
+    <t>Trung tâm chi phí</t>
+  </si>
+  <si>
+    <t>Ngày yêu cầu</t>
+  </si>
+  <si>
+    <t>Hạn xử lý</t>
+  </si>
+  <si>
+    <t>Order Lines/Sản phẩm</t>
+  </si>
+  <si>
+    <t>Order Lines/Mô tả</t>
+  </si>
+  <si>
+    <t>Order Lines/Loại hàng hóa</t>
+  </si>
+  <si>
+    <t>Order Lines/Mô tả tài sản</t>
+  </si>
+  <si>
+    <t>Order Lines/Số lượng đặt mua</t>
+  </si>
+  <si>
+    <t>Order Lines/Số lượng quy đổi</t>
+  </si>
+  <si>
+    <t>Order Lines/Đơn vị mua</t>
+  </si>
+  <si>
+    <t>Order Lines/Số lượng</t>
+  </si>
+  <si>
+    <t>Order Lines/Nhà cung cấp</t>
+  </si>
+  <si>
+    <t>Order Lines/Lệnh sản xuất</t>
+  </si>
+  <si>
+    <t>Order Lines/Trung tâm chi phí</t>
+  </si>
+  <si>
+    <t>Order Lines/Ngày yêu cầu</t>
+  </si>
+  <si>
+    <t>Order Lines/Hạn xử lý</t>
+  </si>
+  <si>
+    <t>Order Lines/Số lượng đã đặt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy;@"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -88,9 +113,10 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -102,14 +128,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor rgb="FF70AD47"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF70AD47"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -122,19 +147,36 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -446,99 +488,120 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="6" width="24.5703125" customWidth="1"/>
-    <col min="7" max="7" width="27" customWidth="1"/>
-    <col min="8" max="8" width="36.5703125" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" customWidth="1"/>
-    <col min="10" max="10" width="25.28515625" customWidth="1"/>
-    <col min="11" max="11" width="27.5703125" customWidth="1"/>
-    <col min="12" max="12" width="25" customWidth="1"/>
-    <col min="13" max="13" width="33.28515625" customWidth="1"/>
-    <col min="14" max="14" width="28.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21" style="6" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="8" customWidth="1"/>
+    <col min="7" max="7" width="15" style="9" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" customWidth="1"/>
+    <col min="10" max="10" width="24.5703125" customWidth="1"/>
+    <col min="11" max="11" width="23.140625" customWidth="1"/>
+    <col min="12" max="12" width="28.85546875" customWidth="1"/>
+    <col min="13" max="13" width="27" customWidth="1"/>
+    <col min="14" max="14" width="23.28515625" customWidth="1"/>
+    <col min="15" max="15" width="19.5703125" customWidth="1"/>
+    <col min="16" max="17" width="23.85546875" customWidth="1"/>
+    <col min="18" max="18" width="30.42578125" customWidth="1"/>
+    <col min="19" max="19" width="25.28515625" customWidth="1"/>
+    <col min="20" max="20" width="21.28515625" customWidth="1"/>
+    <col min="21" max="21" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>10</v>
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="6"/>
+      <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
+      <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="L5" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
quyetnv30 fixbug and update code vss
</commit_message>
<xml_diff>
--- a/addons/custom/purchase_request/static/src/xlsx/template_pr.xlsx
+++ b/addons/custom/purchase_request/static/src/xlsx/template_pr.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECT\erp_forlife\custom_addons\purchase_request\static\src\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\odoo1_6\erp_forlife\custom_addons\purchase_request\static\src\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C670069D-6CF4-4AD1-8CBA-64A74CBB6664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31050" yWindow="4395" windowWidth="22425" windowHeight="11280"/>
+    <workbookView xWindow="32025" yWindow="1200" windowWidth="25545" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Yêu cầu mua hàng" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -24,54 +25,78 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>Department</t>
-  </si>
-  <si>
-    <t>Request date</t>
-  </si>
-  <si>
-    <t>Expected Arrival</t>
-  </si>
-  <si>
-    <t>Order Lines/Product</t>
-  </si>
-  <si>
-    <t>Order Lines/Asset description</t>
-  </si>
-  <si>
-    <t>Order Lines/Quantity Purchase</t>
-  </si>
-  <si>
-    <t>Order Lines/Exchange Quantity</t>
-  </si>
-  <si>
-    <t>Order Lines/UOM Purchase</t>
-  </si>
-  <si>
-    <t>Order Lines/Production Order Code</t>
-  </si>
-  <si>
-    <t>Order Lines/Request date</t>
-  </si>
-  <si>
-    <t>Order Lines/Quantity Order</t>
-  </si>
-  <si>
-    <t>User request</t>
-  </si>
-  <si>
-    <t>Order Lines/Type</t>
-  </si>
-  <si>
-    <t>Order Lines/Vendor</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+  <si>
+    <t>Người yêu cầu</t>
+  </si>
+  <si>
+    <t>Phòng/ban</t>
+  </si>
+  <si>
+    <t>Mã vụ việc</t>
+  </si>
+  <si>
+    <t>Lệnh sản xuất</t>
+  </si>
+  <si>
+    <t>Trung tâm chi phí</t>
+  </si>
+  <si>
+    <t>Ngày yêu cầu</t>
+  </si>
+  <si>
+    <t>Hạn xử lý</t>
+  </si>
+  <si>
+    <t>Order Lines/Sản phẩm</t>
+  </si>
+  <si>
+    <t>Order Lines/Mô tả</t>
+  </si>
+  <si>
+    <t>Order Lines/Loại hàng hóa</t>
+  </si>
+  <si>
+    <t>Order Lines/Mô tả tài sản</t>
+  </si>
+  <si>
+    <t>Order Lines/Số lượng đặt mua</t>
+  </si>
+  <si>
+    <t>Order Lines/Số lượng quy đổi</t>
+  </si>
+  <si>
+    <t>Order Lines/Đơn vị mua</t>
+  </si>
+  <si>
+    <t>Order Lines/Số lượng</t>
+  </si>
+  <si>
+    <t>Order Lines/Nhà cung cấp</t>
+  </si>
+  <si>
+    <t>Order Lines/Lệnh sản xuất</t>
+  </si>
+  <si>
+    <t>Order Lines/Trung tâm chi phí</t>
+  </si>
+  <si>
+    <t>Order Lines/Ngày yêu cầu</t>
+  </si>
+  <si>
+    <t>Order Lines/Hạn xử lý</t>
+  </si>
+  <si>
+    <t>Order Lines/Số lượng đã đặt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy;@"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -88,9 +113,10 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -102,14 +128,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor rgb="FF70AD47"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF70AD47"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -122,19 +147,36 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -446,99 +488,120 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="6" width="24.5703125" customWidth="1"/>
-    <col min="7" max="7" width="27" customWidth="1"/>
-    <col min="8" max="8" width="36.5703125" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" customWidth="1"/>
-    <col min="10" max="10" width="25.28515625" customWidth="1"/>
-    <col min="11" max="11" width="27.5703125" customWidth="1"/>
-    <col min="12" max="12" width="25" customWidth="1"/>
-    <col min="13" max="13" width="33.28515625" customWidth="1"/>
-    <col min="14" max="14" width="28.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21" style="6" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="8" customWidth="1"/>
+    <col min="7" max="7" width="15" style="9" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" customWidth="1"/>
+    <col min="10" max="10" width="24.5703125" customWidth="1"/>
+    <col min="11" max="11" width="23.140625" customWidth="1"/>
+    <col min="12" max="12" width="28.85546875" customWidth="1"/>
+    <col min="13" max="13" width="27" customWidth="1"/>
+    <col min="14" max="14" width="23.28515625" customWidth="1"/>
+    <col min="15" max="15" width="19.5703125" customWidth="1"/>
+    <col min="16" max="17" width="23.85546875" customWidth="1"/>
+    <col min="18" max="18" width="30.42578125" customWidth="1"/>
+    <col min="19" max="19" width="25.28515625" customWidth="1"/>
+    <col min="20" max="20" width="21.28515625" customWidth="1"/>
+    <col min="21" max="21" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>10</v>
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="6"/>
+      <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
+      <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="L5" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Merge branch 'vss' into 'alpha'"
This reverts merge request !274
</commit_message>
<xml_diff>
--- a/addons/custom/purchase_request/static/src/xlsx/template_pr.xlsx
+++ b/addons/custom/purchase_request/static/src/xlsx/template_pr.xlsx
@@ -1,19 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\odoo1_6\erp_forlife\custom_addons\purchase_request\static\src\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECT\erp_forlife\custom_addons\purchase_request\static\src\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C670069D-6CF4-4AD1-8CBA-64A74CBB6664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32025" yWindow="1200" windowWidth="25545" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31050" yWindow="4395" windowWidth="22425" windowHeight="11280"/>
   </bookViews>
   <sheets>
-    <sheet name="Yêu cầu mua hàng" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,78 +24,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
-  <si>
-    <t>Người yêu cầu</t>
-  </si>
-  <si>
-    <t>Phòng/ban</t>
-  </si>
-  <si>
-    <t>Mã vụ việc</t>
-  </si>
-  <si>
-    <t>Lệnh sản xuất</t>
-  </si>
-  <si>
-    <t>Trung tâm chi phí</t>
-  </si>
-  <si>
-    <t>Ngày yêu cầu</t>
-  </si>
-  <si>
-    <t>Hạn xử lý</t>
-  </si>
-  <si>
-    <t>Order Lines/Sản phẩm</t>
-  </si>
-  <si>
-    <t>Order Lines/Mô tả</t>
-  </si>
-  <si>
-    <t>Order Lines/Loại hàng hóa</t>
-  </si>
-  <si>
-    <t>Order Lines/Mô tả tài sản</t>
-  </si>
-  <si>
-    <t>Order Lines/Số lượng đặt mua</t>
-  </si>
-  <si>
-    <t>Order Lines/Số lượng quy đổi</t>
-  </si>
-  <si>
-    <t>Order Lines/Đơn vị mua</t>
-  </si>
-  <si>
-    <t>Order Lines/Số lượng</t>
-  </si>
-  <si>
-    <t>Order Lines/Nhà cung cấp</t>
-  </si>
-  <si>
-    <t>Order Lines/Lệnh sản xuất</t>
-  </si>
-  <si>
-    <t>Order Lines/Trung tâm chi phí</t>
-  </si>
-  <si>
-    <t>Order Lines/Ngày yêu cầu</t>
-  </si>
-  <si>
-    <t>Order Lines/Hạn xử lý</t>
-  </si>
-  <si>
-    <t>Order Lines/Số lượng đã đặt</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Request date</t>
+  </si>
+  <si>
+    <t>Expected Arrival</t>
+  </si>
+  <si>
+    <t>Order Lines/Product</t>
+  </si>
+  <si>
+    <t>Order Lines/Asset description</t>
+  </si>
+  <si>
+    <t>Order Lines/Quantity Purchase</t>
+  </si>
+  <si>
+    <t>Order Lines/Exchange Quantity</t>
+  </si>
+  <si>
+    <t>Order Lines/UOM Purchase</t>
+  </si>
+  <si>
+    <t>Order Lines/Production Order Code</t>
+  </si>
+  <si>
+    <t>Order Lines/Request date</t>
+  </si>
+  <si>
+    <t>Order Lines/Quantity Order</t>
+  </si>
+  <si>
+    <t>User request</t>
+  </si>
+  <si>
+    <t>Order Lines/Type</t>
+  </si>
+  <si>
+    <t>Order Lines/Vendor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy;@"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -113,10 +88,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C5700"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -128,13 +102,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF70AD47"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FF70AD47"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -147,36 +122,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -488,120 +446,99 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" style="6" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" style="8" customWidth="1"/>
-    <col min="7" max="7" width="15" style="9" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" customWidth="1"/>
-    <col min="10" max="10" width="24.5703125" customWidth="1"/>
-    <col min="11" max="11" width="23.140625" customWidth="1"/>
-    <col min="12" max="12" width="28.85546875" customWidth="1"/>
-    <col min="13" max="13" width="27" customWidth="1"/>
-    <col min="14" max="14" width="23.28515625" customWidth="1"/>
-    <col min="15" max="15" width="19.5703125" customWidth="1"/>
-    <col min="16" max="17" width="23.85546875" customWidth="1"/>
-    <col min="18" max="18" width="30.42578125" customWidth="1"/>
-    <col min="19" max="19" width="25.28515625" customWidth="1"/>
-    <col min="20" max="20" width="21.28515625" customWidth="1"/>
-    <col min="21" max="21" width="28.140625" customWidth="1"/>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="6" width="24.5703125" customWidth="1"/>
+    <col min="7" max="7" width="27" customWidth="1"/>
+    <col min="8" max="8" width="36.5703125" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" customWidth="1"/>
+    <col min="10" max="10" width="25.28515625" customWidth="1"/>
+    <col min="11" max="11" width="27.5703125" customWidth="1"/>
+    <col min="12" max="12" width="25" customWidth="1"/>
+    <col min="13" max="13" width="33.28515625" customWidth="1"/>
+    <col min="14" max="14" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
-      <c r="L2" s="3"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="6"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="L3" s="3"/>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
-      <c r="L4" s="3"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="L5" s="3"/>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>